<commit_message>
Added Truong Hong Luu - PI of Bidoup
</commit_message>
<xml_diff>
--- a/ForestGEO_PI_data.xlsx
+++ b/ForestGEO_PI_data.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krizell\Dropbox (Smithsonian)\ForestGEO PI Stats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krizell\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7090"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="469">
   <si>
     <t>Amacayacu</t>
   </si>
@@ -1419,12 +1419,27 @@
   </si>
   <si>
     <t>China, Beijing, Haidian, Xiangshan Rd, 香山路</t>
+  </si>
+  <si>
+    <t>Bidoup</t>
+  </si>
+  <si>
+    <t>Truong Hong Luu</t>
+  </si>
+  <si>
+    <t>lhtruong@sie.vast.vn</t>
+  </si>
+  <si>
+    <t>Southern Institute of Ecology, Vietnam Academy of Science and Technology</t>
+  </si>
+  <si>
+    <t>1 Mac Dinh Chi St., Ward Ben Nghe, 1 Dst., HCM, Viet Nam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -1790,10 +1805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z66"/>
+  <dimension ref="A1:Z67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -2005,32 +2020,24 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>464</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>105</v>
+        <v>465</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>209</v>
+        <v>466</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>452</v>
-      </c>
+        <v>467</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -2038,24 +2045,32 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>230</v>
+        <v>209</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>429</v>
+        <v>451</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+        <v>452</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>452</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -2063,19 +2078,19 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>361</v>
+        <v>429</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>430</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -2088,82 +2103,82 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>233</v>
+        <v>266</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>446</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>448</v>
-      </c>
+        <v>360</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>233</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
+        <v>444</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>232</v>
+        <v>112</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>440</v>
+        <v>449</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -2176,19 +2191,19 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>113</v>
+        <v>441</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>211</v>
+        <v>232</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -2201,19 +2216,19 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -2226,32 +2241,24 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>212</v>
+        <v>239</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>434</v>
-      </c>
+        <v>437</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
@@ -2259,29 +2266,31 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>429</v>
+        <v>435</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G16" s="1"/>
+        <v>116</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H16" s="1" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -2290,31 +2299,29 @@
     </row>
     <row r="17" spans="1:26">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>272</v>
+        <v>231</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>302</v>
+        <v>429</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>303</v>
+        <v>430</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>273</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="G17" s="1"/>
       <c r="H17" s="1" t="s">
-        <v>305</v>
+        <v>431</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>304</v>
+        <v>432</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -2323,24 +2330,32 @@
     </row>
     <row r="18" spans="1:26">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+        <v>303</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>304</v>
+      </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -2348,19 +2363,19 @@
     </row>
     <row r="19" spans="1:26">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>241</v>
+        <v>279</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>411</v>
+        <v>312</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>313</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -2373,19 +2388,19 @@
     </row>
     <row r="20" spans="1:26">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>414</v>
+        <v>410</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>411</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -2398,19 +2413,19 @@
     </row>
     <row r="21" spans="1:26">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -2423,19 +2438,19 @@
     </row>
     <row r="22" spans="1:26">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>267</v>
+        <v>214</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -2448,101 +2463,68 @@
     </row>
     <row r="23" spans="1:26">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="V23" s="6"/>
-      <c r="W23" s="6"/>
-      <c r="X23" s="6"/>
-      <c r="Y23" s="6"/>
-      <c r="Z23" s="6"/>
+        <v>125</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
     </row>
     <row r="24" spans="1:26">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>242</v>
+        <v>67</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>463</v>
+        <v>76</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>243</v>
+        <v>69</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>463</v>
+        <v>74</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>244</v>
+        <v>72</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>409</v>
+        <v>75</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="O24" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="Q24" s="2" t="s">
-        <v>411</v>
+        <v>78</v>
       </c>
       <c r="V24" s="6"/>
       <c r="W24" s="6"/>
@@ -2552,19 +2534,56 @@
     </row>
     <row r="25" spans="1:26">
       <c r="A25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>411</v>
+      </c>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
       <c r="X25" s="6"/>
@@ -2573,32 +2592,15 @@
     </row>
     <row r="26" spans="1:26">
       <c r="A26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>395</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -2611,98 +2613,111 @@
     </row>
     <row r="27" spans="1:26">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>80</v>
+        <v>130</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>82</v>
+        <v>131</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>360</v>
+        <v>396</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>404</v>
-      </c>
+        <v>395</v>
+      </c>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="6"/>
     </row>
     <row r="28" spans="1:26">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>402</v>
+        <v>79</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>406</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>226</v>
+        <v>81</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>396</v>
+        <v>360</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
+        <v>374</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="29" spans="1:26">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="F29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
+        <v>402</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>395</v>
+      </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -2711,365 +2726,355 @@
     </row>
     <row r="30" spans="1:26">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>215</v>
+        <v>257</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="N30" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="O30" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="Q30" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="R30" s="1"/>
+        <v>400</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
     </row>
     <row r="31" spans="1:26">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>292</v>
+        <v>215</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>333</v>
+        <v>393</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>334</v>
+        <v>394</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>293</v>
+        <v>216</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>336</v>
+        <v>396</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>335</v>
+        <v>395</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>334</v>
+        <v>137</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>398</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="P31" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="Q31" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="S31" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="T31" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="U31" s="1" t="s">
-        <v>335</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="R31" s="1"/>
     </row>
     <row r="32" spans="1:26">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="R32" s="1"/>
+        <v>139</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="S32" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="T32" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="U32" s="1" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="33" spans="1:21">
       <c r="A33" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="L33" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>319</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
       <c r="N33" s="1"/>
+      <c r="R33" s="1"/>
     </row>
     <row r="34" spans="1:21">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>258</v>
+        <v>281</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>387</v>
+        <v>316</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>388</v>
+        <v>317</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>390</v>
+        <v>282</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>317</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>260</v>
+        <v>283</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>391</v>
+        <v>318</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>392</v>
+        <v>319</v>
       </c>
       <c r="N34" s="1"/>
-      <c r="R34" s="1"/>
     </row>
     <row r="35" spans="1:21">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
+        <v>390</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>392</v>
+      </c>
       <c r="N35" s="1"/>
       <c r="R35" s="1"/>
     </row>
     <row r="36" spans="1:21">
       <c r="A36" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>287</v>
+        <v>262</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>327</v>
+        <v>383</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>326</v>
+        <v>384</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>288</v>
+        <v>263</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>329</v>
+        <v>385</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="L36" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="M36" s="7" t="s">
-        <v>326</v>
-      </c>
+        <v>386</v>
+      </c>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="R36" s="1"/>
     </row>
     <row r="37" spans="1:21">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>381</v>
+        <v>327</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>382</v>
+        <v>326</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
+        <v>288</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L37" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="M37" s="7" t="s">
+        <v>326</v>
+      </c>
       <c r="N37" s="1"/>
       <c r="R37" s="1"/>
     </row>
     <row r="38" spans="1:21">
       <c r="A38" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>205</v>
+        <v>228</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>81</v>
+        <v>156</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>374</v>
+        <v>229</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>382</v>
       </c>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -3080,23 +3085,32 @@
     </row>
     <row r="39" spans="1:21">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="F39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
+        <v>380</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>374</v>
+      </c>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -3106,19 +3120,19 @@
     </row>
     <row r="40" spans="1:21">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="F40" s="1"/>
       <c r="H40" s="1"/>
@@ -3132,291 +3146,291 @@
     </row>
     <row r="41" spans="1:21">
       <c r="A41" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>374</v>
-      </c>
+        <v>376</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="R41" s="1"/>
     </row>
     <row r="42" spans="1:21">
       <c r="A42" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>240</v>
+        <v>207</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="F42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
+        <v>370</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>374</v>
+      </c>
       <c r="N42" s="1"/>
       <c r="R42" s="1"/>
     </row>
     <row r="43" spans="1:21">
       <c r="A43" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>139</v>
+        <v>162</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>292</v>
+        <v>240</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="L43" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="M43" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="N43" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="O43" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="P43" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="Q43" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="R43" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="S43" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="T43" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="U43" s="1" t="s">
-        <v>335</v>
-      </c>
+        <v>462</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="F43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="R43" s="1"/>
     </row>
     <row r="44" spans="1:21">
       <c r="A44" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>163</v>
+        <v>139</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>221</v>
+        <v>292</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>369</v>
+        <v>333</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>368</v>
+        <v>334</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>164</v>
+        <v>140</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-      <c r="R44" s="1"/>
+        <v>293</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="Q44" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="R44" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="S44" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="T44" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="U44" s="1" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="45" spans="1:21">
       <c r="A45" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
+      <c r="R45" s="1"/>
     </row>
     <row r="46" spans="1:21">
       <c r="A46" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>202</v>
+        <v>223</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="L46" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="M46" s="1" t="s">
-        <v>461</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
       <c r="N46" s="1"/>
-      <c r="R46" s="1"/>
     </row>
     <row r="47" spans="1:21">
       <c r="A47" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>108</v>
+        <v>167</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>266</v>
+        <v>202</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="F47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
+        <v>363</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>461</v>
+      </c>
       <c r="N47" s="1"/>
       <c r="R47" s="1"/>
     </row>
     <row r="48" spans="1:21">
       <c r="A48" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>170</v>
+        <v>108</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>314</v>
+        <v>360</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>315</v>
+        <v>361</v>
       </c>
       <c r="F48" s="1"/>
       <c r="H48" s="1"/>
@@ -3430,32 +3444,23 @@
     </row>
     <row r="49" spans="1:18">
       <c r="A49" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>325</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
@@ -3465,28 +3470,31 @@
     </row>
     <row r="50" spans="1:18">
       <c r="A50" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>225</v>
+        <v>285</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>359</v>
+        <v>322</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>323</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>459</v>
+        <v>172</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>359</v>
+        <v>325</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
@@ -3497,101 +3505,98 @@
     </row>
     <row r="51" spans="1:18">
       <c r="A51" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>269</v>
+        <v>225</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>301</v>
+        <v>459</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>359</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>270</v>
+        <v>174</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="L51" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="M51" s="2" t="s">
-        <v>301</v>
-      </c>
+        <v>459</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
       <c r="N51" s="1"/>
       <c r="R51" s="1"/>
     </row>
     <row r="52" spans="1:18">
       <c r="A52" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>50</v>
+        <v>300</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="F52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
+        <v>301</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>301</v>
+      </c>
       <c r="N52" s="1"/>
       <c r="R52" s="1"/>
     </row>
     <row r="53" spans="1:18">
       <c r="A53" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>357</v>
+        <v>50</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>358</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="F53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
@@ -3601,23 +3606,32 @@
     </row>
     <row r="54" spans="1:18">
       <c r="A54" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="F54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
+        <v>358</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>358</v>
+      </c>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
@@ -3627,97 +3641,88 @@
     </row>
     <row r="55" spans="1:18">
       <c r="A55" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C55" s="1"/>
+        <v>181</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>238</v>
+      </c>
       <c r="D55" s="2" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="J55" s="1" t="s">
-        <v>184</v>
-      </c>
+        <v>356</v>
+      </c>
+      <c r="F55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
       <c r="K55" s="1"/>
-      <c r="L55" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="M55" s="1" t="s">
-        <v>352</v>
-      </c>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
       <c r="N55" s="1"/>
       <c r="R55" s="1"/>
     </row>
     <row r="56" spans="1:18">
       <c r="A56" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>284</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="C56" s="1"/>
       <c r="D56" s="2" t="s">
-        <v>320</v>
+        <v>353</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="F56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
+        <v>354</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>184</v>
+      </c>
       <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
+      <c r="L56" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>352</v>
+      </c>
       <c r="N56" s="1"/>
       <c r="R56" s="1"/>
     </row>
     <row r="57" spans="1:18">
       <c r="A57" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="I57" s="2" t="s">
-        <v>331</v>
-      </c>
+        <v>321</v>
+      </c>
+      <c r="F57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
@@ -3727,23 +3732,32 @@
     </row>
     <row r="58" spans="1:18">
       <c r="A58" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>277</v>
+        <v>290</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="F58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
+        <v>331</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>331</v>
+      </c>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
@@ -3753,109 +3767,100 @@
     </row>
     <row r="59" spans="1:18">
       <c r="A59" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>306</v>
+        <v>332</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="I59" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="J59" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="K59" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="L59" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="M59" s="2" t="s">
-        <v>307</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="F59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
       <c r="N59" s="1"/>
       <c r="R59" s="1"/>
     </row>
     <row r="60" spans="1:18">
       <c r="A60" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>297</v>
+        <v>274</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>339</v>
+        <v>306</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>340</v>
+        <v>307</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
-      <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
+        <v>275</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>307</v>
+      </c>
       <c r="N60" s="1"/>
       <c r="R60" s="1"/>
     </row>
     <row r="61" spans="1:18">
       <c r="A61" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>309</v>
+        <v>297</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>340</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>310</v>
+        <v>341</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>311</v>
+        <v>342</v>
       </c>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
@@ -3866,87 +3871,96 @@
     </row>
     <row r="62" spans="1:18">
       <c r="A62" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>86</v>
+        <v>194</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>277</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>91</v>
+        <v>308</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>92</v>
+        <v>309</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>88</v>
+        <v>195</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>278</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>93</v>
+        <v>310</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="J62" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="K62" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="L62" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M62" s="1" t="s">
-        <v>96</v>
-      </c>
+        <v>311</v>
+      </c>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
       <c r="R62" s="1"/>
     </row>
     <row r="63" spans="1:18">
       <c r="A63" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>227</v>
+        <v>85</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>343</v>
+        <v>91</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
+        <v>92</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K63" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="R63" s="1"/>
     </row>
     <row r="64" spans="1:18">
       <c r="A64" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>261</v>
+        <v>227</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -3956,35 +3970,28 @@
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
+      <c r="R64" s="1"/>
     </row>
     <row r="65" spans="1:13">
       <c r="A65" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>308</v>
+        <v>345</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="I65" s="1" t="s">
-        <v>311</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
@@ -3992,48 +3999,81 @@
     </row>
     <row r="66" spans="1:13">
       <c r="A66" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>249</v>
+        <v>277</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>348</v>
+        <v>308</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>347</v>
+        <v>309</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>250</v>
+        <v>278</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>348</v>
+        <v>310</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>347</v>
+        <v>311</v>
       </c>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
     </row>
+    <row r="67" spans="1:13">
+      <c r="A67" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C23" r:id="rId1" display="mailto:corneilleewango@gmail.com"/>
-    <hyperlink ref="G23" r:id="rId2" display="mailto:jeanremymakana@gmail.com"/>
-    <hyperlink ref="K23" r:id="rId3" display="mailto:terese@bonoboincongo.com"/>
-    <hyperlink ref="C27" r:id="rId4" display="mailto:duncanwt@gmail.com"/>
-    <hyperlink ref="G27" r:id="rId5" display="mailto:kenfackd@si.edu"/>
-    <hyperlink ref="K27" r:id="rId6" display="mailto:Chuyong99@yahoo.com"/>
-    <hyperlink ref="C62" r:id="rId7" display="mailto:michael.morecroft@naturalengland.org.uk"/>
-    <hyperlink ref="G62" r:id="rId8" display="mailto:yadvinder.malhi@ouce.ox.ac.uk"/>
-    <hyperlink ref="K62" r:id="rId9" display="mailto:n.butt@uq.edu.au"/>
+    <hyperlink ref="C24" r:id="rId1" display="mailto:corneilleewango@gmail.com"/>
+    <hyperlink ref="G24" r:id="rId2" display="mailto:jeanremymakana@gmail.com"/>
+    <hyperlink ref="K24" r:id="rId3" display="mailto:terese@bonoboincongo.com"/>
+    <hyperlink ref="C28" r:id="rId4" display="mailto:duncanwt@gmail.com"/>
+    <hyperlink ref="G28" r:id="rId5" display="mailto:kenfackd@si.edu"/>
+    <hyperlink ref="K28" r:id="rId6" display="mailto:Chuyong99@yahoo.com"/>
+    <hyperlink ref="C63" r:id="rId7" display="mailto:michael.morecroft@naturalengland.org.uk"/>
+    <hyperlink ref="G63" r:id="rId8" display="mailto:yadvinder.malhi@ouce.ox.ac.uk"/>
+    <hyperlink ref="K63" r:id="rId9" display="mailto:n.butt@uq.edu.au"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>

</xml_diff>